<commit_message>
Upgrade to PIO 3.8 beta5
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/NewlineInFormulas.xlsx
+++ b/test-data/spreadsheet/NewlineInFormulas.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -349,18 +349,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(
 1,2
 )</f>
         <v>3</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f t="shared" ref="B3:B10" si="0">B1
++B2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
zk-poi upgrade to PIO 3.8 beta5: the rest
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/NewlineInFormulas.xlsx
+++ b/test-data/spreadsheet/NewlineInFormulas.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -349,18 +349,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(
 1,2
 )</f>
         <v>3</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f t="shared" ref="B3:B10" si="0">B1
++B2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>